<commit_message>
UI/UX: Added some backgroung image and linear gradient colors in pages to improve UI
</commit_message>
<xml_diff>
--- a/Format of CA2.xlsx
+++ b/Format of CA2.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\INT219\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asus\Desktop\Full_Stack\Teer_Brand_MERN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{728A52E1-695B-4B11-BB25-6B233990206E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68F0A3D2-080F-416C-995B-768D560C19C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>SNO</t>
   </si>
@@ -49,13 +49,37 @@
   </si>
   <si>
     <t>Video Presentation Link</t>
+  </si>
+  <si>
+    <t>Teer Brand E-commerce Web App</t>
+  </si>
+  <si>
+    <t>CodeSpice</t>
+  </si>
+  <si>
+    <t>INT222</t>
+  </si>
+  <si>
+    <t>Live Link</t>
+  </si>
+  <si>
+    <t>Github Link</t>
+  </si>
+  <si>
+    <t>Youtube Video Presentation</t>
+  </si>
+  <si>
+    <t>Client Approval Form</t>
+  </si>
+  <si>
+    <t>LinkedIn post (This is just post video is uploaded in youtube)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -68,6 +92,14 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -103,18 +135,21 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -447,10 +482,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.09765625" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -460,9 +495,9 @@
     <col min="3" max="3" width="10.796875" style="3"/>
     <col min="4" max="4" width="16.3984375" style="3" customWidth="1"/>
     <col min="5" max="5" width="24.296875" style="3" customWidth="1"/>
-    <col min="6" max="6" width="26.09765625" style="3" customWidth="1"/>
+    <col min="6" max="6" width="49.5" style="3" customWidth="1"/>
     <col min="7" max="7" width="26.296875" style="3" customWidth="1"/>
-    <col min="8" max="8" width="22.19921875" style="3" customWidth="1"/>
+    <col min="8" max="8" width="48.69921875" style="3" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="78" x14ac:dyDescent="0.3">
@@ -491,7 +526,50 @@
         <v>7</v>
       </c>
     </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" s="3">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="3">
+        <v>12307911</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H3" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H4" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="G2" r:id="rId1" xr:uid="{DF693DE6-CEEE-4468-9E55-4230A5791B3E}"/>
+    <hyperlink ref="F2" r:id="rId2" xr:uid="{4DEFCD81-CCDB-434B-8287-7116B57C624E}"/>
+    <hyperlink ref="H2" r:id="rId3" display="LinkedIn post" xr:uid="{7285E352-30DC-4814-8F7E-AE77172BAE9B}"/>
+    <hyperlink ref="H3" r:id="rId4" xr:uid="{A60E8E73-D002-4480-80D0-D53945A43E36}"/>
+    <hyperlink ref="H4" r:id="rId5" xr:uid="{F962AAED-9ECC-4C8B-824E-835DC58D96D2}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>